<commit_message>
Added wikipediaPage, and modified order
</commit_message>
<xml_diff>
--- a/data/Candidates.xlsx
+++ b/data/Candidates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Not.Dropbox\CODING\js_react\candidates\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BC50C0-F39B-4442-971C-1880EF603557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C066E6C-6BD7-4A3F-9661-F8AE909C7B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="-14730" windowWidth="19080" windowHeight="11670" activeTab="1" xr2:uid="{838D9952-C9A6-4E4F-9A32-75481D950E43}"/>
+    <workbookView xWindow="-105" yWindow="-16200" windowWidth="21060" windowHeight="15585" activeTab="1" xr2:uid="{838D9952-C9A6-4E4F-9A32-75481D950E43}"/>
   </bookViews>
   <sheets>
     <sheet name="Criteria" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="101">
   <si>
     <t>RW</t>
   </si>
@@ -315,6 +315,33 @@
   </si>
   <si>
     <t>Independent</t>
+  </si>
+  <si>
+    <t>wikipediaPage</t>
+  </si>
+  <si>
+    <t>Anura_Kumara_Dissanayake</t>
+  </si>
+  <si>
+    <t>A._S._P._Liyanage</t>
+  </si>
+  <si>
+    <t>Janaka_Ratnayake</t>
+  </si>
+  <si>
+    <t>M._A._Sumanthiran</t>
+  </si>
+  <si>
+    <t>Ranil_Wickremesinghe</t>
+  </si>
+  <si>
+    <t>Sarath_Fonseka</t>
+  </si>
+  <si>
+    <t>Sajith_Premadasa</t>
+  </si>
+  <si>
+    <t>Wijeyadasa_Rajapakshe</t>
   </si>
 </sst>
 </file>
@@ -885,24 +912,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7EF6E1-0621-4FD2-8D1B-F60C90A9E974}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" customWidth="1"/>
-    <col min="2" max="2" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>66</v>
       </c>
@@ -916,16 +944,19 @@
         <v>58</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>60</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -939,16 +970,19 @@
         <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
         <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -962,16 +996,19 @@
         <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="F3" t="s">
         <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="H3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -985,16 +1022,19 @@
         <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="F4" t="s">
         <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="H4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1008,16 +1048,19 @@
         <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1031,16 +1074,19 @@
         <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F6" t="s">
         <v>49</v>
       </c>
       <c r="G6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="H6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1054,16 +1100,19 @@
         <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
         <v>53</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="H7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1077,16 +1126,19 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F8" t="s">
         <v>4</v>
       </c>
       <c r="G8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="H8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1100,16 +1152,19 @@
         <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>91</v>
       </c>
       <c r="F9" t="s">
         <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1123,16 +1178,19 @@
         <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="F10" t="s">
         <v>37</v>
       </c>
       <c r="G10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="H10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1146,16 +1204,19 @@
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F11" t="s">
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="H11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1169,17 +1230,20 @@
         <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F12" t="s">
         <v>29</v>
       </c>
       <c r="G12" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="H12" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G12">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F12">
     <sortCondition ref="B2:B12"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
@@ -1195,6 +1259,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>